<commit_message>
pertemuan 10 praktikum 1
</commit_message>
<xml_diff>
--- a/public/template_level.xlsx
+++ b/public/template_level.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28210"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\PWL_POS\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FA7F3B74-091B-4EFC-864C-6784B6360FDA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7006C62-16DC-43EB-91AC-90BFE85C9D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6690" yWindow="3525" windowWidth="15390" windowHeight="7995" xr2:uid="{D09AD215-BC86-4372-8DB0-02BCDD1DE2F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{D09AD215-BC86-4372-8DB0-02BCDD1DE2F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>level_kode</t>
   </si>
@@ -33,16 +33,10 @@
     <t>level_nama</t>
   </si>
   <si>
-    <t>AGT</t>
+    <t>SCR</t>
   </si>
   <si>
-    <t>Agate</t>
-  </si>
-  <si>
-    <t>UNT</t>
-  </si>
-  <si>
-    <t>Unity</t>
+    <t>Security</t>
   </si>
 </sst>
 </file>
@@ -394,10 +388,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91EC98B1-BB63-4991-9AD2-D5CD08BDE7D3}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -422,14 +416,6 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>